<commit_message>
translate system ui to vietnamese
</commit_message>
<xml_diff>
--- a/Lucky-API/wwwroot/uploads/Lucky_Emp_Data.xlsx
+++ b/Lucky-API/wwwroot/uploads/Lucky_Emp_Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\This PC\Downloads\Chrome\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{225015AE-2793-420A-AF4E-4E166C222C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -24,12 +23,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Nguyễn Huỳnh Khánh Vương</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{0D5CF107-ED28-4C7F-88F7-7BA78323BA98}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +42,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{C4C0FDAD-D1B3-473B-A52A-B67BF1B6DD4B}">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{2C487672-B490-4959-95E2-C70B96E246E0}">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -159,7 +158,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="19">
     <font>
       <sz val="11"/>
@@ -800,23 +799,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -852,23 +834,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1044,11 +1009,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>